<commit_message>
feat: integrate Groq LPU for ultra-fast transcription with ffmpeg compression
</commit_message>
<xml_diff>
--- a/docs/test_latenza_rec2pdf_27_11_25.xlsx
+++ b/docs/test_latenza_rec2pdf_27_11_25.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moromoro/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moromoro/Documents/Projects/Rec2pdf/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FB9D28-FF05-0341-91A7-C4033B88962A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F668AF-DF83-4E4A-BEDF-D31EEBDA6864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Scenario</t>
   </si>
@@ -121,10 +121,13 @@
     <t>desktop/mobile</t>
   </si>
   <si>
-    <t>desktop: ok /mobile: HTTP 0</t>
-  </si>
-  <si>
-    <t>desktop: ok /mobile: HTTP 1</t>
+    <t>9 min – web (uploade)</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>14,6 MB</t>
   </si>
 </sst>
 </file>
@@ -189,10 +192,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,16 +508,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
@@ -585,7 +595,7 @@
       <c r="J2">
         <v>1.37</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -620,7 +630,7 @@
       <c r="J3">
         <v>6.62</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -655,7 +665,7 @@
       <c r="J4">
         <v>3.5</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -690,7 +700,7 @@
       <c r="J5">
         <v>5.63</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -725,7 +735,7 @@
       <c r="J6">
         <v>4.1100000000000003</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -734,7 +744,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -760,7 +770,7 @@
       <c r="J7">
         <v>5.8</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -769,7 +779,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -795,8 +805,43 @@
       <c r="J8">
         <v>6.33</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <v>658.21</v>
+      </c>
+      <c r="F9">
+        <v>10.97</v>
+      </c>
+      <c r="G9">
+        <v>90.41</v>
+      </c>
+      <c r="H9">
+        <v>532.5</v>
+      </c>
+      <c r="I9">
+        <v>28.37</v>
+      </c>
+      <c r="J9">
+        <v>6.18</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>